<commit_message>
q9 finished, q8 remains
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musta\Documents\DA8\Projects\budget_lookups-wesiswes629\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11338E54-2997-41BD-92D4-DB4108B09B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCDE381-0263-49EB-920A-C7D5DF2C83D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -787,7 +787,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -830,8 +830,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -843,8 +844,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -884,6 +886,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -2197,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98:G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5825,17 +5828,26 @@
         <f>INDEX($A$1:$P$52,MATCH(B$96,_xlfn.CHOOSECOLS($A$1:$P$52,MATCH(_xlfn.CONCAT($A98,"_",LOWER(LEFT($A$89,4))),$A$1:$P$1,0)),0),MATCH($B$97,_xlfn.CHOOSEROWS($A$1:$P$52,MATCH($B$97,$A$1:$P$1,0)),0))</f>
         <v>Clerk and Master - Chancery</v>
       </c>
-      <c r="C98" s="4"/>
+      <c r="C98" s="9">
+        <f>INDEX($A$1:$P$52,MATCH(B98,$A$1:$A$52,0),MATCH(_xlfn.CONCAT($A98,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>0.15235918433091292</v>
+      </c>
       <c r="D98" t="str">
         <f>INDEX($A$1:$P$52,MATCH(D$96,_xlfn.CHOOSECOLS($A$1:$P$52,MATCH(_xlfn.CONCAT($A98,"_",LOWER(LEFT($A$89,4))),$A$1:$P$1,0)),0),MATCH($B$97,_xlfn.CHOOSEROWS($A$1:$P$52,MATCH($B$97,$A$1:$P$1,0)),0))</f>
         <v>Circuit Court Clerk</v>
       </c>
-      <c r="E98" s="4"/>
+      <c r="E98" s="9">
+        <f>INDEX($A$1:$P$52,MATCH(D98,$A$1:$A$52,0),MATCH(_xlfn.CONCAT($A98,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>0.11502817362571344</v>
+      </c>
       <c r="F98" t="str">
         <f>INDEX($A$1:$P$52,MATCH(F$96,_xlfn.CHOOSECOLS($A$1:$P$52,MATCH(_xlfn.CONCAT($A98,"_",LOWER(LEFT($A$89,4))),$A$1:$P$1,0)),0),MATCH($B$97,_xlfn.CHOOSEROWS($A$1:$P$52,MATCH($B$97,$A$1:$P$1,0)),0))</f>
         <v>Internal Audit</v>
       </c>
-      <c r="G98" s="4"/>
+      <c r="G98" s="9">
+        <f>INDEX($A$1:$P$52,MATCH(F98,$A$1:$A$52,0),5)</f>
+        <v>9.5782760864849215E-2</v>
+      </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
@@ -5846,17 +5858,26 @@
         <f t="shared" ref="B99:F100" si="15">INDEX($A$1:$P$52,MATCH(B$96,_xlfn.CHOOSECOLS($A$1:$P$52,MATCH(_xlfn.CONCAT($A99,"_",LOWER(LEFT($A$89,4))),$A$1:$P$1,0)),0),MATCH($B$97,_xlfn.CHOOSEROWS($A$1:$P$52,MATCH($B$97,$A$1:$P$1,0)),0))</f>
         <v>Metropolitan Clerk</v>
       </c>
-      <c r="C99" s="4"/>
+      <c r="C99" s="9">
+        <f t="shared" ref="C99:C100" si="16">INDEX($A$1:$P$52,MATCH(B99,$A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>0.17551246244575608</v>
+      </c>
       <c r="D99" t="str">
         <f t="shared" si="15"/>
         <v>Internal Audit</v>
       </c>
-      <c r="E99" s="4"/>
+      <c r="E99" s="9">
+        <f t="shared" ref="E99:E100" si="17">INDEX($A$1:$P$52,MATCH(D99,$A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>0.17103239309050916</v>
+      </c>
       <c r="F99" t="str">
         <f t="shared" si="15"/>
         <v>Office of Family Safety</v>
       </c>
-      <c r="G99" s="4"/>
+      <c r="G99" s="9">
+        <f t="shared" ref="G99:G100" si="18">INDEX($A$1:$P$52,MATCH(F99,$A$1:$A$52,0),5)</f>
+        <v>8.008952370177623E-2</v>
+      </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -5867,17 +5888,26 @@
         <f t="shared" si="15"/>
         <v>Community Oversight Board</v>
       </c>
-      <c r="C100" s="4"/>
+      <c r="C100" s="9">
+        <f t="shared" si="16"/>
+        <v>0.82994157333333329</v>
+      </c>
       <c r="D100" t="str">
         <f t="shared" si="15"/>
         <v>Clerk and Master - Chancery</v>
       </c>
-      <c r="E100" s="4"/>
+      <c r="E100" s="9">
+        <f t="shared" si="17"/>
+        <v>0.15295680364719175</v>
+      </c>
       <c r="F100" t="str">
         <f t="shared" si="15"/>
         <v>Election Commission</v>
       </c>
-      <c r="G100" s="4"/>
+      <c r="G100" s="9">
+        <f t="shared" si="18"/>
+        <v>5.4037002206391245E-2</v>
+      </c>
       <c r="I100" s="4"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
@@ -5885,266 +5915,435 @@
         <f>_xlfn.CONCAT(A91,"_",LOWER(LEFT(A89,4)))</f>
         <v>FY17_rank</v>
       </c>
+      <c r="C104" t="str">
+        <f>_xlfn.CONCAT(A98,"_diff_pct")</f>
+        <v>FY17_diff_pct</v>
+      </c>
+      <c r="D104">
+        <f>MATCH(B98,A1:A52,0)</f>
+        <v>8</v>
+      </c>
+      <c r="E104">
+        <f>MATCH(C104,A1:P1,0)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B105" t="str" cm="1">
         <f t="array" ref="B105:B156">_xlfn.CHOOSECOLS(A1:P52,MATCH(B104,A1:P1,0))</f>
         <v>FY17_rank</v>
       </c>
+      <c r="C105" t="str" cm="1">
+        <f t="array" ref="C105:C156">_xlfn.CHOOSECOLS(B1:Q52,MATCH(C104,B1:Q1,0))</f>
+        <v>FY17_diff_pct</v>
+      </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B106">
         <v>14</v>
       </c>
+      <c r="C106">
+        <v>4.3170750765267295E-2</v>
+      </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B107">
         <v>22</v>
       </c>
+      <c r="C107">
+        <v>2.3069981751824741E-2</v>
+      </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B108">
         <v>42</v>
       </c>
+      <c r="C108">
+        <v>4.9327413275443007E-3</v>
+      </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B109">
         <v>4</v>
       </c>
+      <c r="C109">
+        <v>9.4273968477453174E-2</v>
+      </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B110">
         <v>11</v>
       </c>
+      <c r="C110">
+        <v>5.7149963352064452E-2</v>
+      </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B111">
         <v>2</v>
       </c>
+      <c r="C111">
+        <v>0.11502817362571344</v>
+      </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C112">
+        <v>0.15235918433091292</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B113">
         <v>16</v>
       </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C113">
+        <v>4.2417130511048909E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B114">
         <v>6</v>
       </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C114">
+        <v>8.1681998646514792E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B115">
         <v>47</v>
       </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B116">
         <v>13</v>
       </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C116">
+        <v>5.0060657805601608E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B117">
         <v>33</v>
       </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C117">
+        <v>1.2912833886247806E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B118">
         <v>30</v>
       </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C118">
+        <v>1.3637949218750009E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B119">
         <v>51</v>
       </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C119">
+        <v>-3.1837408866824991E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B120">
         <v>37</v>
       </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C120">
+        <v>1.1850188616360429E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B121">
         <v>21</v>
       </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C121">
+        <v>2.8351094826658003E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B122">
         <v>12</v>
       </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C122">
+        <v>5.4037002206391245E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B123">
         <v>15</v>
       </c>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C123">
+        <v>4.258504294298146E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B124">
         <v>46</v>
       </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C124">
+        <v>1.2379538203300809E-5</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B125">
         <v>9</v>
       </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C125">
+        <v>7.9052463618023094E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B126">
         <v>32</v>
       </c>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C126">
+        <v>1.3285502334437123E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B127">
         <v>18</v>
       </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C127">
+        <v>3.9590110100806722E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B128">
         <v>31</v>
       </c>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C128">
+        <v>1.3334943305713101E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B129">
         <v>38</v>
       </c>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C129">
+        <v>1.0226130964676661E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B130">
         <v>5</v>
       </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C130">
+        <v>8.5306091660634673E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B131">
         <v>47</v>
       </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B132">
         <v>3</v>
       </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C132">
+        <v>9.5782760864849215E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B133">
         <v>28</v>
       </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C133">
+        <v>1.4800253727847622E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B134">
         <v>40</v>
       </c>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C134">
+        <v>8.3831374359143746E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B135">
         <v>29</v>
       </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C135">
+        <v>1.4030533529678329E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B136">
         <v>36</v>
       </c>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C136">
+        <v>1.2294942827617691E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B137">
         <v>41</v>
       </c>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C137">
+        <v>7.9969930789269058E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B138">
         <v>26</v>
       </c>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C138">
+        <v>1.8939149738619768E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B139">
         <v>47</v>
       </c>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B140">
         <v>10</v>
       </c>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C140">
+        <v>7.8647857679780775E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B141">
         <v>19</v>
       </c>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C141">
+        <v>3.9444515758219188E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B142">
         <v>25</v>
       </c>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C142">
+        <v>1.9443680579913542E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B143">
         <v>8</v>
       </c>
-    </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C143">
+        <v>8.008952370177623E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B144">
         <v>23</v>
       </c>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C144">
+        <v>2.1279773539092578E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B145">
         <v>17</v>
       </c>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C145">
+        <v>4.0110550149132493E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B146">
         <v>44</v>
       </c>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C146">
+        <v>2.2070943135841053E-4</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B147">
         <v>24</v>
       </c>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C147">
+        <v>2.0497353541313264E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B148">
         <v>39</v>
       </c>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C148">
+        <v>9.7760750186150751E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B149">
         <v>34</v>
       </c>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C149">
+        <v>1.287514194887851E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B150">
         <v>43</v>
       </c>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C150">
+        <v>3.0010420686993711E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B151">
         <v>45</v>
       </c>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C151">
+        <v>1.7435939690898361E-4</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B152">
         <v>20</v>
       </c>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C152">
+        <v>3.1133192323107857E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B153">
         <v>27</v>
       </c>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C153">
+        <v>1.8444360086767971E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B154">
         <v>47</v>
       </c>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B155">
         <v>35</v>
       </c>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C155">
+        <v>1.2785255822058129E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B156">
         <v>7</v>
+      </c>
+      <c r="C156">
+        <v>8.009596083231342E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>